<commit_message>
actualizar test sprint 3
</commit_message>
<xml_diff>
--- a/testing/Grupo_4_-_Testing_Proyecto_Final_-_Sprint_III.xlsx
+++ b/testing/Grupo_4_-_Testing_Proyecto_Final_-_Sprint_III.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cff67f99b37eafb7/Documentos/DH/Proyecto Integrador/grupo-04/testing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="164" documentId="11_B8DD8B580280C79DE2433FE5189BAD30D1B21B29" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A106C48C-78AF-4749-A5FE-D33F51A86480}"/>
+  <xr:revisionPtr revIDLastSave="177" documentId="11_B8DD8B580280C79DE2433FE5189BAD30D1B21B29" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B3C36395-2B7D-4F1E-AA1F-6DFED6483164}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-4815" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Casos de Prueba" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="253">
   <si>
     <t>Id</t>
   </si>
@@ -1240,6 +1240,84 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1259,108 +1337,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFEA4335"/>
-          <bgColor rgb="FFEA4335"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFEA4335"/>
-          <bgColor rgb="FFEA4335"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1580,8 +1563,8 @@
   </sheetPr>
   <dimension ref="A1:I58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24:H58"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="H54" sqref="H54:H58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1599,33 +1582,33 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="7"/>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="15"/>
+      <c r="G1" s="41"/>
       <c r="H1" s="9"/>
-      <c r="I1" s="14" t="s">
+      <c r="I1" s="40" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="7"/>
-      <c r="B2" s="20"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
       <c r="F2" s="8" t="s">
         <v>6</v>
       </c>
@@ -1635,10 +1618,10 @@
       <c r="H2" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="15"/>
+      <c r="I2" s="41"/>
     </row>
     <row r="3" spans="1:9" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="44" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="10" t="s">
@@ -1667,7 +1650,7 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A4" s="19"/>
+      <c r="A4" s="45"/>
       <c r="B4" s="10" t="s">
         <v>24</v>
       </c>
@@ -1694,7 +1677,7 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A5" s="19"/>
+      <c r="A5" s="45"/>
       <c r="B5" s="10" t="s">
         <v>25</v>
       </c>
@@ -1721,7 +1704,7 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A6" s="19"/>
+      <c r="A6" s="45"/>
       <c r="B6" s="10" t="s">
         <v>26</v>
       </c>
@@ -1748,7 +1731,7 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A7" s="19"/>
+      <c r="A7" s="45"/>
       <c r="B7" s="10" t="s">
         <v>27</v>
       </c>
@@ -1802,7 +1785,7 @@
       </c>
     </row>
     <row r="9" spans="1:9" ht="102" x14ac:dyDescent="0.2">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="42" t="s">
         <v>72</v>
       </c>
       <c r="B9" s="10" t="s">
@@ -1831,7 +1814,7 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="140.25" x14ac:dyDescent="0.2">
-      <c r="A10" s="17"/>
+      <c r="A10" s="43"/>
       <c r="B10" s="10" t="s">
         <v>137</v>
       </c>
@@ -1858,7 +1841,7 @@
       </c>
     </row>
     <row r="11" spans="1:9" ht="114.75" x14ac:dyDescent="0.2">
-      <c r="A11" s="17"/>
+      <c r="A11" s="43"/>
       <c r="B11" s="10" t="s">
         <v>138</v>
       </c>
@@ -1885,7 +1868,7 @@
       </c>
     </row>
     <row r="12" spans="1:9" ht="140.25" x14ac:dyDescent="0.2">
-      <c r="A12" s="17"/>
+      <c r="A12" s="43"/>
       <c r="B12" s="10" t="s">
         <v>139</v>
       </c>
@@ -1912,7 +1895,7 @@
       </c>
     </row>
     <row r="13" spans="1:9" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A13" s="17"/>
+      <c r="A13" s="43"/>
       <c r="B13" s="10" t="s">
         <v>140</v>
       </c>
@@ -1939,7 +1922,7 @@
       </c>
     </row>
     <row r="14" spans="1:9" ht="114.75" x14ac:dyDescent="0.2">
-      <c r="A14" s="17"/>
+      <c r="A14" s="43"/>
       <c r="B14" s="10" t="s">
         <v>141</v>
       </c>
@@ -1966,7 +1949,7 @@
       </c>
     </row>
     <row r="15" spans="1:9" ht="114.75" x14ac:dyDescent="0.2">
-      <c r="A15" s="17"/>
+      <c r="A15" s="43"/>
       <c r="B15" s="10" t="s">
         <v>142</v>
       </c>
@@ -1993,7 +1976,7 @@
       </c>
     </row>
     <row r="16" spans="1:9" ht="178.5" x14ac:dyDescent="0.2">
-      <c r="A16" s="17"/>
+      <c r="A16" s="43"/>
       <c r="B16" s="10" t="s">
         <v>143</v>
       </c>
@@ -2020,7 +2003,7 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="178.5" x14ac:dyDescent="0.2">
-      <c r="A17" s="17"/>
+      <c r="A17" s="43"/>
       <c r="B17" s="10" t="s">
         <v>144</v>
       </c>
@@ -2047,7 +2030,7 @@
       </c>
     </row>
     <row r="18" spans="1:9" ht="178.5" x14ac:dyDescent="0.2">
-      <c r="A18" s="17"/>
+      <c r="A18" s="43"/>
       <c r="B18" s="10" t="s">
         <v>145</v>
       </c>
@@ -2074,7 +2057,7 @@
       </c>
     </row>
     <row r="19" spans="1:9" ht="178.5" x14ac:dyDescent="0.2">
-      <c r="A19" s="17"/>
+      <c r="A19" s="43"/>
       <c r="B19" s="10" t="s">
         <v>146</v>
       </c>
@@ -2101,7 +2084,7 @@
       </c>
     </row>
     <row r="20" spans="1:9" ht="178.5" x14ac:dyDescent="0.2">
-      <c r="A20" s="17"/>
+      <c r="A20" s="43"/>
       <c r="B20" s="10" t="s">
         <v>147</v>
       </c>
@@ -2128,7 +2111,7 @@
       </c>
     </row>
     <row r="21" spans="1:9" ht="140.25" x14ac:dyDescent="0.2">
-      <c r="A21" s="17"/>
+      <c r="A21" s="43"/>
       <c r="B21" s="10" t="s">
         <v>148</v>
       </c>
@@ -2155,7 +2138,7 @@
       </c>
     </row>
     <row r="22" spans="1:9" ht="102" x14ac:dyDescent="0.2">
-      <c r="A22" s="17"/>
+      <c r="A22" s="43"/>
       <c r="B22" s="10" t="s">
         <v>149</v>
       </c>
@@ -2182,7 +2165,7 @@
       </c>
     </row>
     <row r="23" spans="1:9" ht="102" x14ac:dyDescent="0.2">
-      <c r="A23" s="17"/>
+      <c r="A23" s="43"/>
       <c r="B23" s="10" t="s">
         <v>150</v>
       </c>
@@ -2209,679 +2192,738 @@
       </c>
     </row>
     <row r="24" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A24" s="25" t="s">
+      <c r="A24" s="30" t="s">
         <v>227</v>
       </c>
       <c r="B24" s="23" t="s">
         <v>228</v>
       </c>
-      <c r="C24" s="21" t="s">
+      <c r="C24" s="32" t="s">
         <v>159</v>
       </c>
-      <c r="D24" s="21" t="s">
+      <c r="D24" s="32" t="s">
         <v>160</v>
       </c>
-      <c r="E24" s="26" t="s">
+      <c r="E24" s="39" t="s">
         <v>161</v>
       </c>
-      <c r="F24" s="27" t="s">
+      <c r="F24" s="15" t="s">
         <v>162</v>
       </c>
-      <c r="G24" s="28" t="s">
+      <c r="G24" s="16" t="s">
         <v>163</v>
       </c>
-      <c r="H24" s="33"/>
-      <c r="I24" s="35" t="s">
+      <c r="H24" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="I24" s="36" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A25" s="29"/>
+      <c r="A25" s="31"/>
       <c r="B25" s="24"/>
-      <c r="C25" s="30"/>
-      <c r="D25" s="30"/>
-      <c r="E25" s="30"/>
-      <c r="F25" s="28" t="s">
+      <c r="C25" s="27"/>
+      <c r="D25" s="27"/>
+      <c r="E25" s="27"/>
+      <c r="F25" s="16" t="s">
         <v>164</v>
       </c>
-      <c r="G25" s="28" t="s">
+      <c r="G25" s="16" t="s">
         <v>165</v>
       </c>
-      <c r="H25" s="34"/>
-      <c r="I25" s="36"/>
+      <c r="H25" s="35"/>
+      <c r="I25" s="38"/>
     </row>
     <row r="26" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A26" s="29"/>
+      <c r="A26" s="31"/>
       <c r="B26" s="23" t="s">
         <v>229</v>
       </c>
-      <c r="C26" s="21" t="s">
+      <c r="C26" s="32" t="s">
         <v>166</v>
       </c>
-      <c r="D26" s="21" t="s">
+      <c r="D26" s="32" t="s">
         <v>167</v>
       </c>
-      <c r="E26" s="26" t="s">
+      <c r="E26" s="39" t="s">
         <v>161</v>
       </c>
-      <c r="F26" s="28" t="s">
+      <c r="F26" s="16" t="s">
         <v>168</v>
       </c>
-      <c r="G26" s="28" t="s">
+      <c r="G26" s="16" t="s">
         <v>163</v>
       </c>
-      <c r="H26" s="33"/>
-      <c r="I26" s="35" t="s">
+      <c r="H26" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="I26" s="36" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A27" s="29"/>
+      <c r="A27" s="31"/>
       <c r="B27" s="24"/>
-      <c r="C27" s="30"/>
-      <c r="D27" s="30"/>
-      <c r="E27" s="30"/>
-      <c r="F27" s="28" t="s">
+      <c r="C27" s="27"/>
+      <c r="D27" s="27"/>
+      <c r="E27" s="27"/>
+      <c r="F27" s="16" t="s">
         <v>164</v>
       </c>
-      <c r="G27" s="28" t="s">
+      <c r="G27" s="16" t="s">
         <v>169</v>
       </c>
-      <c r="H27" s="34"/>
-      <c r="I27" s="36"/>
+      <c r="H27" s="35"/>
+      <c r="I27" s="38"/>
     </row>
     <row r="28" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A28" s="29"/>
+      <c r="A28" s="31"/>
       <c r="B28" s="23" t="s">
         <v>230</v>
       </c>
-      <c r="C28" s="21" t="s">
+      <c r="C28" s="32" t="s">
         <v>170</v>
       </c>
-      <c r="D28" s="21" t="s">
+      <c r="D28" s="32" t="s">
         <v>171</v>
       </c>
-      <c r="E28" s="21" t="s">
+      <c r="E28" s="32" t="s">
         <v>172</v>
       </c>
-      <c r="F28" s="28" t="s">
+      <c r="F28" s="16" t="s">
         <v>173</v>
       </c>
-      <c r="G28" s="28" t="s">
+      <c r="G28" s="16" t="s">
         <v>174</v>
       </c>
-      <c r="H28" s="33"/>
-      <c r="I28" s="35" t="s">
+      <c r="H28" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="I28" s="36" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="51" x14ac:dyDescent="0.2">
-      <c r="A29" s="29"/>
+      <c r="A29" s="31"/>
       <c r="B29" s="24"/>
-      <c r="C29" s="30"/>
-      <c r="D29" s="30"/>
-      <c r="E29" s="30"/>
-      <c r="F29" s="28" t="s">
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="16" t="s">
         <v>175</v>
       </c>
-      <c r="G29" s="28" t="s">
+      <c r="G29" s="16" t="s">
         <v>176</v>
       </c>
-      <c r="H29" s="34"/>
-      <c r="I29" s="36"/>
+      <c r="H29" s="35"/>
+      <c r="I29" s="38"/>
     </row>
     <row r="30" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A30" s="29"/>
+      <c r="A30" s="31"/>
       <c r="B30" s="23" t="s">
         <v>231</v>
       </c>
-      <c r="C30" s="21" t="s">
+      <c r="C30" s="32" t="s">
         <v>177</v>
       </c>
-      <c r="D30" s="21" t="s">
+      <c r="D30" s="32" t="s">
         <v>178</v>
       </c>
-      <c r="E30" s="21" t="s">
+      <c r="E30" s="32" t="s">
         <v>170</v>
       </c>
-      <c r="F30" s="28" t="s">
+      <c r="F30" s="16" t="s">
         <v>173</v>
       </c>
-      <c r="G30" s="28" t="s">
+      <c r="G30" s="16" t="s">
         <v>174</v>
       </c>
-      <c r="H30" s="33"/>
-      <c r="I30" s="35" t="s">
+      <c r="H30" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="I30" s="36" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A31" s="29"/>
+      <c r="A31" s="31"/>
       <c r="B31" s="24"/>
-      <c r="C31" s="30"/>
-      <c r="D31" s="30"/>
-      <c r="E31" s="30"/>
-      <c r="F31" s="28" t="s">
+      <c r="C31" s="27"/>
+      <c r="D31" s="27"/>
+      <c r="E31" s="27"/>
+      <c r="F31" s="16" t="s">
         <v>175</v>
       </c>
-      <c r="G31" s="28" t="s">
+      <c r="G31" s="16" t="s">
         <v>179</v>
       </c>
-      <c r="H31" s="34"/>
-      <c r="I31" s="36"/>
+      <c r="H31" s="35"/>
+      <c r="I31" s="38"/>
     </row>
     <row r="32" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A32" s="29"/>
+      <c r="A32" s="31"/>
       <c r="B32" s="23" t="s">
         <v>232</v>
       </c>
-      <c r="C32" s="21" t="s">
+      <c r="C32" s="32" t="s">
         <v>180</v>
       </c>
-      <c r="D32" s="21" t="s">
+      <c r="D32" s="32" t="s">
         <v>181</v>
       </c>
-      <c r="E32" s="21" t="s">
+      <c r="E32" s="32" t="s">
         <v>182</v>
       </c>
-      <c r="F32" s="27" t="s">
+      <c r="F32" s="15" t="s">
         <v>183</v>
       </c>
-      <c r="G32" s="28" t="s">
+      <c r="G32" s="16" t="s">
         <v>184</v>
       </c>
-      <c r="H32" s="33"/>
-      <c r="I32" s="35" t="s">
+      <c r="H32" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="I32" s="36" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A33" s="29"/>
+      <c r="A33" s="31"/>
       <c r="B33" s="24"/>
-      <c r="C33" s="30"/>
-      <c r="D33" s="30"/>
-      <c r="E33" s="30"/>
-      <c r="F33" s="28" t="s">
+      <c r="C33" s="27"/>
+      <c r="D33" s="27"/>
+      <c r="E33" s="27"/>
+      <c r="F33" s="16" t="s">
         <v>185</v>
       </c>
-      <c r="G33" s="28" t="s">
+      <c r="G33" s="16" t="s">
         <v>186</v>
       </c>
-      <c r="H33" s="34"/>
-      <c r="I33" s="36"/>
+      <c r="H33" s="35"/>
+      <c r="I33" s="38"/>
     </row>
     <row r="34" spans="1:9" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A34" s="29"/>
+      <c r="A34" s="31"/>
       <c r="B34" s="23" t="s">
         <v>233</v>
       </c>
-      <c r="C34" s="21" t="s">
+      <c r="C34" s="32" t="s">
         <v>187</v>
       </c>
-      <c r="D34" s="21" t="s">
+      <c r="D34" s="32" t="s">
         <v>188</v>
       </c>
-      <c r="E34" s="21" t="s">
+      <c r="E34" s="32" t="s">
         <v>189</v>
       </c>
-      <c r="F34" s="27" t="s">
+      <c r="F34" s="15" t="s">
         <v>190</v>
       </c>
-      <c r="G34" s="28" t="s">
+      <c r="G34" s="16" t="s">
         <v>191</v>
       </c>
-      <c r="H34" s="33"/>
-      <c r="I34" s="35" t="s">
+      <c r="H34" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="I34" s="36" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A35" s="29"/>
+      <c r="A35" s="31"/>
       <c r="B35" s="24"/>
-      <c r="C35" s="30"/>
-      <c r="D35" s="30"/>
-      <c r="E35" s="30"/>
-      <c r="F35" s="28" t="s">
+      <c r="C35" s="27"/>
+      <c r="D35" s="27"/>
+      <c r="E35" s="27"/>
+      <c r="F35" s="16" t="s">
         <v>192</v>
       </c>
-      <c r="G35" s="28" t="s">
+      <c r="G35" s="16" t="s">
         <v>193</v>
       </c>
-      <c r="H35" s="34"/>
-      <c r="I35" s="36"/>
+      <c r="H35" s="35"/>
+      <c r="I35" s="38"/>
     </row>
     <row r="36" spans="1:9" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A36" s="29"/>
-      <c r="B36" s="39" t="s">
+      <c r="A36" s="31"/>
+      <c r="B36" s="25" t="s">
         <v>234</v>
       </c>
-      <c r="C36" s="21" t="s">
+      <c r="C36" s="32" t="s">
         <v>194</v>
       </c>
-      <c r="D36" s="21" t="s">
+      <c r="D36" s="32" t="s">
         <v>195</v>
       </c>
-      <c r="E36" s="21" t="s">
+      <c r="E36" s="32" t="s">
         <v>189</v>
       </c>
-      <c r="F36" s="27" t="s">
+      <c r="F36" s="15" t="s">
         <v>196</v>
       </c>
-      <c r="G36" s="28" t="s">
+      <c r="G36" s="16" t="s">
         <v>191</v>
       </c>
-      <c r="H36" s="33"/>
-      <c r="I36" s="35" t="s">
+      <c r="H36" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="I36" s="36" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A37" s="29"/>
-      <c r="B37" s="31"/>
-      <c r="C37" s="31"/>
-      <c r="D37" s="31"/>
-      <c r="E37" s="31"/>
-      <c r="F37" s="28" t="s">
+      <c r="A37" s="31"/>
+      <c r="B37" s="26"/>
+      <c r="C37" s="26"/>
+      <c r="D37" s="26"/>
+      <c r="E37" s="26"/>
+      <c r="F37" s="16" t="s">
         <v>197</v>
       </c>
-      <c r="G37" s="28" t="s">
+      <c r="G37" s="16" t="s">
         <v>198</v>
       </c>
-      <c r="H37" s="37"/>
-      <c r="I37" s="38"/>
+      <c r="H37" s="34"/>
+      <c r="I37" s="37"/>
     </row>
     <row r="38" spans="1:9" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A38" s="29"/>
-      <c r="B38" s="30"/>
-      <c r="C38" s="30"/>
-      <c r="D38" s="30"/>
-      <c r="E38" s="30"/>
-      <c r="F38" s="28" t="s">
+      <c r="A38" s="31"/>
+      <c r="B38" s="27"/>
+      <c r="C38" s="27"/>
+      <c r="D38" s="27"/>
+      <c r="E38" s="27"/>
+      <c r="F38" s="16" t="s">
         <v>192</v>
       </c>
-      <c r="G38" s="28" t="s">
+      <c r="G38" s="16" t="s">
         <v>199</v>
       </c>
-      <c r="H38" s="34"/>
-      <c r="I38" s="36"/>
+      <c r="H38" s="35"/>
+      <c r="I38" s="38"/>
     </row>
     <row r="39" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A39" s="29"/>
-      <c r="B39" s="39" t="s">
+      <c r="A39" s="31"/>
+      <c r="B39" s="25" t="s">
         <v>235</v>
       </c>
-      <c r="C39" s="21" t="s">
+      <c r="C39" s="32" t="s">
         <v>200</v>
       </c>
-      <c r="D39" s="21" t="s">
+      <c r="D39" s="32" t="s">
         <v>201</v>
       </c>
-      <c r="E39" s="21" t="s">
+      <c r="E39" s="32" t="s">
         <v>202</v>
       </c>
-      <c r="F39" s="27" t="s">
+      <c r="F39" s="15" t="s">
         <v>173</v>
       </c>
-      <c r="G39" s="28" t="s">
+      <c r="G39" s="16" t="s">
         <v>174</v>
       </c>
-      <c r="H39" s="33"/>
-      <c r="I39" s="35" t="s">
+      <c r="H39" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="I39" s="36" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="51" x14ac:dyDescent="0.2">
-      <c r="A40" s="29"/>
-      <c r="B40" s="31"/>
-      <c r="C40" s="31"/>
-      <c r="D40" s="31"/>
-      <c r="E40" s="31"/>
-      <c r="F40" s="28" t="s">
+      <c r="A40" s="31"/>
+      <c r="B40" s="26"/>
+      <c r="C40" s="26"/>
+      <c r="D40" s="26"/>
+      <c r="E40" s="26"/>
+      <c r="F40" s="16" t="s">
         <v>175</v>
       </c>
-      <c r="G40" s="28" t="s">
+      <c r="G40" s="16" t="s">
         <v>176</v>
       </c>
-      <c r="H40" s="37"/>
-      <c r="I40" s="38"/>
+      <c r="H40" s="34"/>
+      <c r="I40" s="37"/>
     </row>
     <row r="41" spans="1:9" ht="102" x14ac:dyDescent="0.2">
-      <c r="A41" s="29"/>
-      <c r="B41" s="30"/>
-      <c r="C41" s="30"/>
-      <c r="D41" s="30"/>
-      <c r="E41" s="30"/>
-      <c r="F41" s="28" t="s">
+      <c r="A41" s="31"/>
+      <c r="B41" s="27"/>
+      <c r="C41" s="27"/>
+      <c r="D41" s="27"/>
+      <c r="E41" s="27"/>
+      <c r="F41" s="16" t="s">
         <v>203</v>
       </c>
-      <c r="G41" s="28" t="s">
+      <c r="G41" s="16" t="s">
         <v>204</v>
       </c>
-      <c r="H41" s="34"/>
-      <c r="I41" s="36"/>
+      <c r="H41" s="35"/>
+      <c r="I41" s="38"/>
     </row>
     <row r="42" spans="1:9" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A42" s="29"/>
-      <c r="B42" s="39" t="s">
+      <c r="A42" s="31"/>
+      <c r="B42" s="25" t="s">
         <v>236</v>
       </c>
-      <c r="C42" s="21" t="s">
+      <c r="C42" s="32" t="s">
         <v>205</v>
       </c>
-      <c r="D42" s="21" t="s">
+      <c r="D42" s="32" t="s">
         <v>206</v>
       </c>
-      <c r="E42" s="21" t="s">
+      <c r="E42" s="32" t="s">
         <v>207</v>
       </c>
-      <c r="F42" s="27" t="s">
+      <c r="F42" s="15" t="s">
         <v>208</v>
       </c>
-      <c r="G42" s="28" t="s">
+      <c r="G42" s="16" t="s">
         <v>191</v>
       </c>
-      <c r="H42" s="33"/>
-      <c r="I42" s="35" t="s">
+      <c r="H42" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="I42" s="36" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="102" x14ac:dyDescent="0.2">
-      <c r="A43" s="29"/>
-      <c r="B43" s="31"/>
-      <c r="C43" s="31"/>
-      <c r="D43" s="31"/>
-      <c r="E43" s="31"/>
-      <c r="F43" s="28" t="s">
+      <c r="A43" s="31"/>
+      <c r="B43" s="26"/>
+      <c r="C43" s="26"/>
+      <c r="D43" s="26"/>
+      <c r="E43" s="26"/>
+      <c r="F43" s="16" t="s">
         <v>203</v>
       </c>
-      <c r="G43" s="28" t="s">
+      <c r="G43" s="16" t="s">
         <v>204</v>
       </c>
-      <c r="H43" s="37"/>
-      <c r="I43" s="38"/>
+      <c r="H43" s="34"/>
+      <c r="I43" s="37"/>
     </row>
     <row r="44" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A44" s="29"/>
-      <c r="B44" s="30"/>
-      <c r="C44" s="30"/>
-      <c r="D44" s="30"/>
-      <c r="E44" s="30"/>
-      <c r="F44" s="28" t="s">
+      <c r="A44" s="31"/>
+      <c r="B44" s="27"/>
+      <c r="C44" s="27"/>
+      <c r="D44" s="27"/>
+      <c r="E44" s="27"/>
+      <c r="F44" s="16" t="s">
         <v>209</v>
       </c>
-      <c r="G44" s="28" t="s">
+      <c r="G44" s="16" t="s">
         <v>210</v>
       </c>
-      <c r="H44" s="34"/>
-      <c r="I44" s="36"/>
+      <c r="H44" s="35"/>
+      <c r="I44" s="38"/>
     </row>
     <row r="45" spans="1:9" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A45" s="29"/>
-      <c r="B45" s="42" t="s">
+      <c r="A45" s="31"/>
+      <c r="B45" s="18" t="s">
         <v>237</v>
       </c>
-      <c r="C45" s="22" t="s">
+      <c r="C45" s="14" t="s">
         <v>211</v>
       </c>
-      <c r="D45" s="22" t="s">
+      <c r="D45" s="14" t="s">
         <v>212</v>
       </c>
-      <c r="E45" s="22" t="s">
+      <c r="E45" s="14" t="s">
         <v>213</v>
       </c>
-      <c r="F45" s="32" t="s">
+      <c r="F45" s="17" t="s">
         <v>214</v>
       </c>
-      <c r="G45" s="28" t="s">
+      <c r="G45" s="16" t="s">
         <v>215</v>
       </c>
-      <c r="H45" s="10"/>
+      <c r="H45" s="10" t="s">
+        <v>50</v>
+      </c>
       <c r="I45" s="10" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="46" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A46" s="29"/>
-      <c r="B46" s="39" t="s">
+      <c r="A46" s="31"/>
+      <c r="B46" s="25" t="s">
         <v>238</v>
       </c>
-      <c r="C46" s="21" t="s">
+      <c r="C46" s="32" t="s">
         <v>216</v>
       </c>
-      <c r="D46" s="21" t="s">
+      <c r="D46" s="32" t="s">
         <v>217</v>
       </c>
-      <c r="E46" s="21" t="s">
+      <c r="E46" s="32" t="s">
         <v>200</v>
       </c>
-      <c r="F46" s="28" t="s">
+      <c r="F46" s="16" t="s">
         <v>173</v>
       </c>
-      <c r="G46" s="28" t="s">
+      <c r="G46" s="16" t="s">
         <v>174</v>
       </c>
-      <c r="H46" s="33"/>
-      <c r="I46" s="35" t="s">
+      <c r="H46" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="I46" s="36" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="47" spans="1:9" ht="51" x14ac:dyDescent="0.2">
-      <c r="A47" s="29"/>
-      <c r="B47" s="40"/>
-      <c r="C47" s="31"/>
-      <c r="D47" s="31"/>
-      <c r="E47" s="31"/>
-      <c r="F47" s="28" t="s">
+      <c r="A47" s="31"/>
+      <c r="B47" s="28"/>
+      <c r="C47" s="26"/>
+      <c r="D47" s="26"/>
+      <c r="E47" s="26"/>
+      <c r="F47" s="16" t="s">
         <v>175</v>
       </c>
-      <c r="G47" s="28" t="s">
+      <c r="G47" s="16" t="s">
         <v>176</v>
       </c>
-      <c r="H47" s="37"/>
-      <c r="I47" s="38"/>
+      <c r="H47" s="34"/>
+      <c r="I47" s="37"/>
     </row>
     <row r="48" spans="1:9" ht="102" x14ac:dyDescent="0.2">
-      <c r="A48" s="29"/>
-      <c r="B48" s="40"/>
-      <c r="C48" s="31"/>
-      <c r="D48" s="31"/>
-      <c r="E48" s="31"/>
-      <c r="F48" s="28" t="s">
+      <c r="A48" s="31"/>
+      <c r="B48" s="28"/>
+      <c r="C48" s="26"/>
+      <c r="D48" s="26"/>
+      <c r="E48" s="26"/>
+      <c r="F48" s="16" t="s">
         <v>203</v>
       </c>
-      <c r="G48" s="28" t="s">
+      <c r="G48" s="16" t="s">
         <v>204</v>
       </c>
-      <c r="H48" s="37"/>
-      <c r="I48" s="38"/>
+      <c r="H48" s="34"/>
+      <c r="I48" s="37"/>
     </row>
     <row r="49" spans="1:9" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A49" s="29"/>
-      <c r="B49" s="41"/>
-      <c r="C49" s="30"/>
-      <c r="D49" s="30"/>
-      <c r="E49" s="30"/>
-      <c r="F49" s="28" t="s">
+      <c r="A49" s="31"/>
+      <c r="B49" s="29"/>
+      <c r="C49" s="27"/>
+      <c r="D49" s="27"/>
+      <c r="E49" s="27"/>
+      <c r="F49" s="16" t="s">
         <v>218</v>
       </c>
-      <c r="G49" s="28" t="s">
+      <c r="G49" s="16" t="s">
         <v>219</v>
       </c>
-      <c r="H49" s="34"/>
-      <c r="I49" s="36"/>
+      <c r="H49" s="35"/>
+      <c r="I49" s="38"/>
     </row>
     <row r="50" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A50" s="29"/>
-      <c r="B50" s="39" t="s">
+      <c r="A50" s="31"/>
+      <c r="B50" s="25" t="s">
         <v>239</v>
       </c>
-      <c r="C50" s="21" t="s">
+      <c r="C50" s="32" t="s">
         <v>220</v>
       </c>
-      <c r="D50" s="21" t="s">
+      <c r="D50" s="32" t="s">
         <v>221</v>
       </c>
-      <c r="E50" s="21" t="s">
+      <c r="E50" s="32" t="s">
         <v>207</v>
       </c>
-      <c r="F50" s="27" t="s">
+      <c r="F50" s="15" t="s">
         <v>173</v>
       </c>
-      <c r="G50" s="28" t="s">
+      <c r="G50" s="16" t="s">
         <v>174</v>
       </c>
-      <c r="H50" s="33"/>
-      <c r="I50" s="35" t="s">
+      <c r="H50" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="I50" s="36" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="51" spans="1:9" ht="51" x14ac:dyDescent="0.2">
-      <c r="A51" s="29"/>
-      <c r="B51" s="40"/>
-      <c r="C51" s="31"/>
-      <c r="D51" s="31"/>
-      <c r="E51" s="31"/>
-      <c r="F51" s="28" t="s">
+      <c r="A51" s="31"/>
+      <c r="B51" s="28"/>
+      <c r="C51" s="26"/>
+      <c r="D51" s="26"/>
+      <c r="E51" s="26"/>
+      <c r="F51" s="16" t="s">
         <v>175</v>
       </c>
-      <c r="G51" s="28" t="s">
+      <c r="G51" s="16" t="s">
         <v>176</v>
       </c>
-      <c r="H51" s="37"/>
-      <c r="I51" s="38"/>
+      <c r="H51" s="34"/>
+      <c r="I51" s="37"/>
     </row>
     <row r="52" spans="1:9" ht="102" x14ac:dyDescent="0.2">
-      <c r="A52" s="29"/>
-      <c r="B52" s="40"/>
-      <c r="C52" s="31"/>
-      <c r="D52" s="31"/>
-      <c r="E52" s="31"/>
-      <c r="F52" s="28" t="s">
+      <c r="A52" s="31"/>
+      <c r="B52" s="28"/>
+      <c r="C52" s="26"/>
+      <c r="D52" s="26"/>
+      <c r="E52" s="26"/>
+      <c r="F52" s="16" t="s">
         <v>203</v>
       </c>
-      <c r="G52" s="28" t="s">
+      <c r="G52" s="16" t="s">
         <v>204</v>
       </c>
-      <c r="H52" s="37"/>
-      <c r="I52" s="38"/>
+      <c r="H52" s="34"/>
+      <c r="I52" s="37"/>
     </row>
     <row r="53" spans="1:9" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A53" s="29"/>
-      <c r="B53" s="41"/>
-      <c r="C53" s="30"/>
-      <c r="D53" s="30"/>
-      <c r="E53" s="30"/>
-      <c r="F53" s="28" t="s">
+      <c r="A53" s="31"/>
+      <c r="B53" s="29"/>
+      <c r="C53" s="27"/>
+      <c r="D53" s="27"/>
+      <c r="E53" s="27"/>
+      <c r="F53" s="16" t="s">
         <v>218</v>
       </c>
-      <c r="G53" s="28" t="s">
+      <c r="G53" s="16" t="s">
         <v>219</v>
       </c>
-      <c r="H53" s="34"/>
-      <c r="I53" s="36"/>
+      <c r="H53" s="35"/>
+      <c r="I53" s="38"/>
     </row>
     <row r="54" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A54" s="29"/>
-      <c r="B54" s="39" t="s">
+      <c r="A54" s="31"/>
+      <c r="B54" s="25" t="s">
         <v>240</v>
       </c>
-      <c r="C54" s="21" t="s">
+      <c r="C54" s="32" t="s">
         <v>222</v>
       </c>
-      <c r="D54" s="21" t="s">
+      <c r="D54" s="32" t="s">
         <v>223</v>
       </c>
-      <c r="E54" s="21" t="s">
+      <c r="E54" s="32" t="s">
         <v>224</v>
       </c>
-      <c r="F54" s="27" t="s">
+      <c r="F54" s="15" t="s">
         <v>173</v>
       </c>
-      <c r="G54" s="28" t="s">
+      <c r="G54" s="16" t="s">
         <v>174</v>
       </c>
-      <c r="H54" s="33"/>
-      <c r="I54" s="35" t="s">
+      <c r="H54" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="I54" s="36" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="55" spans="1:9" ht="51" x14ac:dyDescent="0.2">
-      <c r="A55" s="29"/>
-      <c r="B55" s="31"/>
-      <c r="C55" s="31"/>
-      <c r="D55" s="31"/>
-      <c r="E55" s="31"/>
-      <c r="F55" s="28" t="s">
+      <c r="A55" s="31"/>
+      <c r="B55" s="26"/>
+      <c r="C55" s="26"/>
+      <c r="D55" s="26"/>
+      <c r="E55" s="26"/>
+      <c r="F55" s="16" t="s">
         <v>175</v>
       </c>
-      <c r="G55" s="28" t="s">
+      <c r="G55" s="16" t="s">
         <v>176</v>
       </c>
-      <c r="H55" s="37"/>
-      <c r="I55" s="38"/>
+      <c r="H55" s="34"/>
+      <c r="I55" s="37"/>
     </row>
     <row r="56" spans="1:9" ht="102" x14ac:dyDescent="0.2">
-      <c r="A56" s="29"/>
-      <c r="B56" s="31"/>
-      <c r="C56" s="31"/>
-      <c r="D56" s="31"/>
-      <c r="E56" s="31"/>
-      <c r="F56" s="28" t="s">
+      <c r="A56" s="31"/>
+      <c r="B56" s="26"/>
+      <c r="C56" s="26"/>
+      <c r="D56" s="26"/>
+      <c r="E56" s="26"/>
+      <c r="F56" s="16" t="s">
         <v>203</v>
       </c>
-      <c r="G56" s="28" t="s">
+      <c r="G56" s="16" t="s">
         <v>204</v>
       </c>
-      <c r="H56" s="37"/>
-      <c r="I56" s="38"/>
+      <c r="H56" s="34"/>
+      <c r="I56" s="37"/>
     </row>
     <row r="57" spans="1:9" ht="89.25" x14ac:dyDescent="0.2">
-      <c r="A57" s="29"/>
-      <c r="B57" s="31"/>
-      <c r="C57" s="31"/>
-      <c r="D57" s="31"/>
-      <c r="E57" s="31"/>
-      <c r="F57" s="28" t="s">
+      <c r="A57" s="31"/>
+      <c r="B57" s="26"/>
+      <c r="C57" s="26"/>
+      <c r="D57" s="26"/>
+      <c r="E57" s="26"/>
+      <c r="F57" s="16" t="s">
         <v>218</v>
       </c>
-      <c r="G57" s="28" t="s">
+      <c r="G57" s="16" t="s">
         <v>219</v>
       </c>
-      <c r="H57" s="37"/>
-      <c r="I57" s="38"/>
+      <c r="H57" s="34"/>
+      <c r="I57" s="37"/>
     </row>
     <row r="58" spans="1:9" ht="51" x14ac:dyDescent="0.2">
-      <c r="A58" s="29"/>
-      <c r="B58" s="30"/>
-      <c r="C58" s="30"/>
-      <c r="D58" s="30"/>
-      <c r="E58" s="30"/>
-      <c r="F58" s="28" t="s">
+      <c r="A58" s="31"/>
+      <c r="B58" s="27"/>
+      <c r="C58" s="27"/>
+      <c r="D58" s="27"/>
+      <c r="E58" s="27"/>
+      <c r="F58" s="16" t="s">
         <v>225</v>
       </c>
-      <c r="G58" s="28" t="s">
+      <c r="G58" s="16" t="s">
         <v>226</v>
       </c>
-      <c r="H58" s="34"/>
-      <c r="I58" s="36"/>
+      <c r="H58" s="35"/>
+      <c r="I58" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="81">
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="B39:B41"/>
-    <mergeCell ref="B42:B44"/>
-    <mergeCell ref="B46:B49"/>
-    <mergeCell ref="B50:B53"/>
-    <mergeCell ref="B54:B58"/>
-    <mergeCell ref="A24:A58"/>
-    <mergeCell ref="C54:C58"/>
-    <mergeCell ref="D54:D58"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="A9:A23"/>
+    <mergeCell ref="A3:A7"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="H26:H27"/>
+    <mergeCell ref="I26:I27"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="H24:H25"/>
+    <mergeCell ref="I24:I25"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="H30:H31"/>
+    <mergeCell ref="I30:I31"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="H28:H29"/>
+    <mergeCell ref="I28:I29"/>
+    <mergeCell ref="E34:E35"/>
+    <mergeCell ref="H34:H35"/>
+    <mergeCell ref="I34:I35"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="E32:E33"/>
+    <mergeCell ref="H32:H33"/>
+    <mergeCell ref="I32:I33"/>
+    <mergeCell ref="E39:E41"/>
+    <mergeCell ref="H39:H41"/>
+    <mergeCell ref="I39:I41"/>
+    <mergeCell ref="C36:C38"/>
+    <mergeCell ref="D36:D38"/>
+    <mergeCell ref="E36:E38"/>
+    <mergeCell ref="H36:H38"/>
+    <mergeCell ref="I36:I38"/>
+    <mergeCell ref="E46:E49"/>
+    <mergeCell ref="H46:H49"/>
+    <mergeCell ref="I46:I49"/>
+    <mergeCell ref="C42:C44"/>
+    <mergeCell ref="D42:D44"/>
+    <mergeCell ref="E42:E44"/>
+    <mergeCell ref="H42:H44"/>
+    <mergeCell ref="I42:I44"/>
     <mergeCell ref="E54:E58"/>
     <mergeCell ref="H54:H58"/>
     <mergeCell ref="I54:I58"/>
@@ -2890,64 +2932,31 @@
     <mergeCell ref="E50:E53"/>
     <mergeCell ref="H50:H53"/>
     <mergeCell ref="I50:I53"/>
+    <mergeCell ref="B50:B53"/>
+    <mergeCell ref="B54:B58"/>
+    <mergeCell ref="A24:A58"/>
+    <mergeCell ref="C54:C58"/>
+    <mergeCell ref="D54:D58"/>
     <mergeCell ref="C46:C49"/>
     <mergeCell ref="D46:D49"/>
-    <mergeCell ref="E46:E49"/>
-    <mergeCell ref="H46:H49"/>
-    <mergeCell ref="I46:I49"/>
-    <mergeCell ref="C42:C44"/>
-    <mergeCell ref="D42:D44"/>
-    <mergeCell ref="E42:E44"/>
-    <mergeCell ref="H42:H44"/>
-    <mergeCell ref="I42:I44"/>
     <mergeCell ref="C39:C41"/>
     <mergeCell ref="D39:D41"/>
-    <mergeCell ref="E39:E41"/>
-    <mergeCell ref="H39:H41"/>
-    <mergeCell ref="I39:I41"/>
-    <mergeCell ref="C36:C38"/>
-    <mergeCell ref="D36:D38"/>
-    <mergeCell ref="E36:E38"/>
-    <mergeCell ref="H36:H38"/>
-    <mergeCell ref="I36:I38"/>
     <mergeCell ref="C34:C35"/>
     <mergeCell ref="D34:D35"/>
-    <mergeCell ref="E34:E35"/>
-    <mergeCell ref="H34:H35"/>
-    <mergeCell ref="I34:I35"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="E32:E33"/>
-    <mergeCell ref="H32:H33"/>
-    <mergeCell ref="I32:I33"/>
     <mergeCell ref="C30:C31"/>
     <mergeCell ref="D30:D31"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="H30:H31"/>
-    <mergeCell ref="I30:I31"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="H28:H29"/>
-    <mergeCell ref="I28:I29"/>
     <mergeCell ref="C26:C27"/>
     <mergeCell ref="D26:D27"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="H26:H27"/>
-    <mergeCell ref="I26:I27"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="H24:H25"/>
-    <mergeCell ref="I24:I25"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="A9:A23"/>
-    <mergeCell ref="A3:A7"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="B42:B44"/>
+    <mergeCell ref="B46:B49"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="B32:B33"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3077,131 +3086,131 @@
     <col min="6" max="16384" width="11.42578125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="6" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A1" s="43" t="s">
+    <row r="1" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A1" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="43" t="s">
+      <c r="C1" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="43" t="s">
+      <c r="D1" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="43" t="s">
+      <c r="E1" s="19" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="44" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="B2" s="44" t="s">
+      <c r="B2" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="C2" s="44" t="s">
+      <c r="C2" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="D2" s="44"/>
-      <c r="E2" s="45" t="s">
+      <c r="D2" s="20"/>
+      <c r="E2" s="21" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="44" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="B3" s="44" t="s">
+      <c r="B3" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="C3" s="44" t="s">
+      <c r="C3" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="D3" s="44"/>
-      <c r="E3" s="45" t="s">
+      <c r="D3" s="20"/>
+      <c r="E3" s="21" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="44" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="B4" s="44" t="s">
+      <c r="B4" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="C4" s="44" t="s">
+      <c r="C4" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="D4" s="44"/>
-      <c r="E4" s="45" t="s">
+      <c r="D4" s="20"/>
+      <c r="E4" s="21" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="44" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="B5" s="44" t="s">
+      <c r="B5" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="C5" s="44" t="s">
+      <c r="C5" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="D5" s="44"/>
-      <c r="E5" s="45" t="s">
+      <c r="D5" s="20"/>
+      <c r="E5" s="21" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="44" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="20" t="s">
         <v>153</v>
       </c>
-      <c r="B6" s="44" t="s">
+      <c r="B6" s="20" t="s">
         <v>155</v>
       </c>
-      <c r="C6" s="44" t="s">
+      <c r="C6" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="D6" s="44"/>
-      <c r="E6" s="45" t="s">
+      <c r="D6" s="20"/>
+      <c r="E6" s="21" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="6" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A7" s="44" t="s">
+    <row r="7" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A7" s="20" t="s">
         <v>154</v>
       </c>
-      <c r="B7" s="44" t="s">
+      <c r="B7" s="20" t="s">
         <v>156</v>
       </c>
-      <c r="C7" s="44" t="s">
+      <c r="C7" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="D7" s="44"/>
-      <c r="E7" s="45" t="s">
+      <c r="D7" s="20"/>
+      <c r="E7" s="21" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="44" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="20" t="s">
         <v>246</v>
       </c>
-      <c r="B8" s="46" t="s">
+      <c r="B8" s="22" t="s">
         <v>241</v>
       </c>
-      <c r="C8" s="44"/>
-      <c r="D8" s="44"/>
-      <c r="E8" s="45" t="s">
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="21" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="44" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="20" t="s">
         <v>247</v>
       </c>
-      <c r="B9" s="46" t="s">
+      <c r="B9" s="22" t="s">
         <v>243</v>
       </c>
       <c r="C9" s="13"/>
@@ -3210,11 +3219,11 @@
         <v>250</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="44" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="20" t="s">
         <v>248</v>
       </c>
-      <c r="B10" s="46" t="s">
+      <c r="B10" s="22" t="s">
         <v>244</v>
       </c>
       <c r="C10" s="13"/>
@@ -3223,11 +3232,11 @@
         <v>251</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="44" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="20" t="s">
         <v>249</v>
       </c>
-      <c r="B11" s="46" t="s">
+      <c r="B11" s="22" t="s">
         <v>245</v>
       </c>
       <c r="C11" s="13"/>

</xml_diff>